<commit_message>
data manip, save to csv
</commit_message>
<xml_diff>
--- a/datadescriptive.xlsx
+++ b/datadescriptive.xlsx
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>63.50669165309886</v>
+        <v>63.51691476969101</v>
       </c>
       <c r="C3" t="n">
         <v>1066.499085427028</v>
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>25.85747668063898</v>
+        <v>25.8285177638053</v>
       </c>
       <c r="C4" t="n">
-        <v>509.6281056181521</v>
+        <v>509.6281056181531</v>
       </c>
       <c r="D4" t="n">
-        <v>96.25514278043227</v>
+        <v>96.25514278043239</v>
       </c>
       <c r="E4" t="n">
-        <v>1037.069513617561</v>
+        <v>1037.069513617562</v>
       </c>
     </row>
     <row r="5">
@@ -519,7 +519,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-37.63000106811523</v>
+        <v>10.01000022888184</v>
       </c>
       <c r="C5" t="n">
         <v>255.1000061035156</v>

</xml_diff>